<commit_message>
Add best exam and worst exam for evaluating multiple bugs in BankAccountTP system
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/Summary/BankAccountTP/multiple_bugs_123bug.xlsx
+++ b/experiment_results/SBFL_ONLY/Summary/BankAccountTP/multiple_bugs_123bug.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="9">
   <si>
     <t>EVALUATION_METRIC</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Worst rank</t>
+  </si>
+  <si>
+    <t>Best exam</t>
+  </si>
+  <si>
+    <t>Worst exam</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -514,6 +520,22 @@
         <v>16.83289817232376</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>6.523762226400829</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.75520932085312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -521,7 +543,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -640,6 +662,22 @@
         <v>14.80939947780679</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.041909397216465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.13158851453251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -647,7 +685,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,6 +804,22 @@
         <v>15.44647519582245</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.186112652487536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.96867188627947</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -773,7 +827,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -892,6 +946,22 @@
         <v>16.10182767624021</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.743342558398804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.83463069876829</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -899,7 +969,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1018,6 +1088,22 @@
         <v>16.10182767624021</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.743342558398804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.83463069876829</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1025,7 +1111,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1144,6 +1230,22 @@
         <v>15.73629242819843</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.725236265466182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.33644237175215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1151,7 +1253,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1270,6 +1372,22 @@
         <v>16.42819843342037</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.406070452596446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.20927214755002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1277,7 +1395,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1396,6 +1514,22 @@
         <v>20.92689295039164</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>10.67334570686556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>26.99384048580321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1403,7 +1537,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1522,6 +1656,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1529,7 +1679,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1648,6 +1798,22 @@
         <v>14.80939947780679</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.041909397216465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.13158851453251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1655,7 +1821,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1774,6 +1940,22 @@
         <v>14.80939947780679</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.041909397216465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.13158851453251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1781,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1900,6 +2082,22 @@
         <v>15.34986945169713</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.685184637569725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.82851293219664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1907,7 +2105,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2026,6 +2224,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,7 +2247,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2152,6 +2366,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2159,7 +2389,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2278,6 +2508,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2285,7 +2531,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2404,6 +2650,22 @@
         <v>16.21148825065274</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.266201992405422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.93808653239007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2411,7 +2673,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2530,6 +2792,22 @@
         <v>15.73368146214099</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.909404174414617</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.32374413576328</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2537,7 +2815,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2656,6 +2934,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2663,7 +2957,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2782,6 +3076,22 @@
         <v>16.75718015665796</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.52808136612143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.68362953853219</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2789,7 +3099,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2908,6 +3218,22 @@
         <v>14.80939947780679</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.041909397216465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.13158851453251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2915,7 +3241,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3034,6 +3360,22 @@
         <v>14.80939947780679</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.041909397216465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>19.13158851453251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3041,7 +3383,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3160,6 +3502,22 @@
         <v>15.93211488250653</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.909404174414617</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.58092690164781</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3167,7 +3525,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3286,6 +3644,22 @@
         <v>16.4934725848564</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.327431842653215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.29711610884301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3293,7 +3667,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3412,6 +3786,22 @@
         <v>16.42819843342037</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>4.246646708982527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.21749121125517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3419,7 +3809,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3538,6 +3928,22 @@
         <v>16.8355091383812</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>6.530633189709885</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>21.75864480250765</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3545,7 +3951,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3664,6 +4070,22 @@
         <v>15.66579634464752</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.760243388654732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20.23220377015845</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3671,7 +4093,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3790,6 +4212,22 @@
         <v>20.92689295039164</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>10.67334570686556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>26.99384048580321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3797,7 +4235,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3916,6 +4354,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3923,7 +4377,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4042,6 +4496,22 @@
         <v>41.78067885117493</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20.31487276541489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>54.23551400893749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4049,7 +4519,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4168,6 +4638,22 @@
         <v>22.10443864229765</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.800077581003437</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>28.61773613065617</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>